<commit_message>
AP-23036: Add tests for ExcelFormat and WriteWorkbookHandler methods
Change creator metadata in XLSX test file to "KNIME Testauthor"
so that is different from the "Apache POI" default value.

AP-23036 (Excel Writer writes unnecessary metadata which is flagged as sensitive by PowerBI)
</commit_message>
<xml_diff>
--- a/org.knime.ext.poi3.tests/files/unencrypted.xlsx
+++ b/org.knime.ext.poi3.tests/files/unencrypted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manuelhotz/git/master/kap/knime-excel/org.knime.ext.poi3.tests/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:8001_{A3139D1C-56FD-3349-9CDD-8AB959C1CBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C354B13-0274-9648-B9F3-405C4CFA9518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="5360" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="knime" sheetId="8" r:id="rId1"/>
@@ -51,6 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,9 +101,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -140,7 +141,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -246,7 +247,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -388,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -405,37 +406,37 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>6</v>
       </c>
     </row>
@@ -456,37 +457,37 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>90</v>
       </c>
     </row>

</xml_diff>